<commit_message>
Redefine the time covariate for the roe deer data
</commit_message>
<xml_diff>
--- a/tables/model_summaries_non_park_comparison.xlsx
+++ b/tables/model_summaries_non_park_comparison.xlsx
@@ -441,13 +441,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>1.5006</v>
+        <v>2.1328</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5203</v>
+        <v>0.3086</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0039</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -455,13 +455,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.367</v>
+        <v>0.3513</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1751</v>
+        <v>0.1754</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0361</v>
+        <v>0.0452</v>
       </c>
     </row>
     <row r="4">
@@ -469,13 +469,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.1614</v>
+        <v>-0.1743</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3012</v>
+        <v>0.2995</v>
       </c>
       <c r="D4" t="n">
-        <v>0.592</v>
+        <v>0.5607</v>
       </c>
     </row>
     <row r="5">
@@ -483,13 +483,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3008</v>
+        <v>0.2866</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1811</v>
+        <v>0.1815</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0967</v>
+        <v>0.1144</v>
       </c>
     </row>
     <row r="6">
@@ -497,13 +497,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.3088</v>
+        <v>-0.315</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5905</v>
+        <v>0.5718</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6009</v>
+        <v>0.5817</v>
       </c>
     </row>
     <row r="7">
@@ -511,13 +511,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.4023</v>
+        <v>0.3802</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1892</v>
+        <v>0.1914</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0335</v>
+        <v>0.0469</v>
       </c>
     </row>
     <row r="8">
@@ -525,13 +525,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>0.14</v>
+        <v>0.1454</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1864</v>
+        <v>0.1871</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4526</v>
+        <v>0.4372</v>
       </c>
     </row>
     <row r="9">
@@ -539,13 +539,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.2809</v>
+        <v>-0.2981</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5956</v>
+        <v>0.5973</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6372</v>
+        <v>0.6177</v>
       </c>
     </row>
     <row r="10">
@@ -553,13 +553,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.3463</v>
+        <v>0.354</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2742</v>
+        <v>0.3412</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2065</v>
+        <v>0.2995</v>
       </c>
     </row>
     <row r="11">
@@ -567,13 +567,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1975</v>
+        <v>-0.0462</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2795</v>
+        <v>0.2272</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4798</v>
+        <v>0.8387</v>
       </c>
     </row>
     <row r="12">
@@ -581,13 +581,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.39</v>
+        <v>-0.0662</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4221</v>
+        <v>0.2904</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3555</v>
+        <v>0.8197</v>
       </c>
     </row>
     <row r="13">
@@ -595,13 +595,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>0.5138</v>
+        <v>0.0049</v>
       </c>
       <c r="C13" t="n">
-        <v>0.4714</v>
+        <v>0.2811</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2758</v>
+        <v>0.9861</v>
       </c>
     </row>
     <row r="14">
@@ -609,13 +609,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>0.5614</v>
+        <v>0.0034</v>
       </c>
       <c r="C14" t="n">
-        <v>0.4883</v>
+        <v>0.2631</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2503</v>
+        <v>0.9898</v>
       </c>
     </row>
     <row r="15">
@@ -623,13 +623,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>0.5573</v>
+        <v>-0.095</v>
       </c>
       <c r="C15" t="n">
-        <v>0.504</v>
+        <v>0.2623</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2689</v>
+        <v>0.717</v>
       </c>
     </row>
     <row r="16">
@@ -637,13 +637,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>0.5876</v>
+        <v>-0.137</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5081</v>
+        <v>0.2822</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2474</v>
+        <v>0.6273</v>
       </c>
     </row>
     <row r="17">
@@ -651,13 +651,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.6515</v>
+        <v>-0.1825</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5046</v>
+        <v>0.3264</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1967</v>
+        <v>0.5761</v>
       </c>
     </row>
     <row r="18">
@@ -665,13 +665,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>0.5901</v>
+        <v>-0.2675</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5024</v>
+        <v>0.3789</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2402</v>
+        <v>0.4803</v>
       </c>
     </row>
     <row r="19">
@@ -679,13 +679,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>0.4991</v>
+        <v>-0.297</v>
       </c>
       <c r="C19" t="n">
-        <v>0.5016</v>
+        <v>0.4097</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3198</v>
+        <v>0.4685</v>
       </c>
     </row>
     <row r="20">
@@ -693,13 +693,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>0.5167</v>
+        <v>-0.245</v>
       </c>
       <c r="C20" t="n">
-        <v>0.4917</v>
+        <v>0.4323</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2933</v>
+        <v>0.5709</v>
       </c>
     </row>
     <row r="21">
@@ -707,13 +707,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>0.6117</v>
+        <v>-0.2255</v>
       </c>
       <c r="C21" t="n">
-        <v>0.4973</v>
+        <v>0.4906</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2186</v>
+        <v>0.6458</v>
       </c>
     </row>
     <row r="22">
@@ -721,13 +721,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>0.7204</v>
+        <v>-0.2132</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6068</v>
+        <v>0.6461</v>
       </c>
       <c r="D22" t="n">
-        <v>0.2351</v>
+        <v>0.7415</v>
       </c>
     </row>
     <row r="23">
@@ -735,10 +735,10 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-1.3215</v>
+        <v>-1.3204</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0803</v>
+        <v>0.0809</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -777,105 +777,125 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>10.8778</v>
+        <v>-1.05</v>
       </c>
       <c r="C2" t="n">
-        <v>12.7466</v>
+        <v>6.8395</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3934</v>
+        <v>0.878</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3"/>
+      <c r="B3" t="n">
+        <v>-2.7078</v>
+      </c>
       <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3"/>
+        <v>52520.9888</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.4866</v>
+        <v>0.5188</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3391</v>
+        <v>0.3428</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1512</v>
+        <v>0.1301</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" t="n">
+        <v>-2.7081</v>
+      </c>
       <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5"/>
+        <v>61907.51</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.3978</v>
+        <v>0.4167</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3188</v>
+        <v>0.3232</v>
       </c>
       <c r="D6" t="n">
-        <v>0.212</v>
+        <v>0.1973</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7"/>
+      <c r="B7" t="n">
+        <v>-1.5612</v>
+      </c>
       <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7"/>
+        <v>68203.7739</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" t="n">
+        <v>-3.0336</v>
+      </c>
       <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8"/>
+        <v>58893.6987</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9"/>
+      <c r="B9" t="n">
+        <v>-2.9034</v>
+      </c>
       <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9"/>
+        <v>74191.5672</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-6.361</v>
+        <v>0.048</v>
       </c>
       <c r="C10" t="n">
-        <v>10.8758</v>
+        <v>0.9843</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5586</v>
+        <v>0.9611</v>
       </c>
     </row>
     <row r="11">
@@ -883,13 +903,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-2.9097</v>
+        <v>0.4391</v>
       </c>
       <c r="C11" t="n">
-        <v>2.9619</v>
+        <v>3.125</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3259</v>
+        <v>0.8883</v>
       </c>
     </row>
     <row r="12">
@@ -897,13 +917,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-5.582</v>
+        <v>0.8782</v>
       </c>
       <c r="C12" t="n">
-        <v>5.05</v>
+        <v>5.3822</v>
       </c>
       <c r="D12" t="n">
-        <v>0.269</v>
+        <v>0.8704</v>
       </c>
     </row>
     <row r="13">
@@ -911,13 +931,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-7.6948</v>
+        <v>1.3151</v>
       </c>
       <c r="C13" t="n">
-        <v>7.2608</v>
+        <v>6.6563</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2892</v>
+        <v>0.8434</v>
       </c>
     </row>
     <row r="14">
@@ -925,13 +945,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-9.2431</v>
+        <v>1.7624</v>
       </c>
       <c r="C14" t="n">
-        <v>9.4241</v>
+        <v>6.9234</v>
       </c>
       <c r="D14" t="n">
-        <v>0.3267</v>
+        <v>0.7991</v>
       </c>
     </row>
     <row r="15">
@@ -939,13 +959,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-10.2268</v>
+        <v>2.03</v>
       </c>
       <c r="C15" t="n">
-        <v>11.2768</v>
+        <v>6.8475</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3645</v>
+        <v>0.7669</v>
       </c>
     </row>
     <row r="16">
@@ -953,13 +973,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-10.6459</v>
+        <v>2.2062</v>
       </c>
       <c r="C16" t="n">
-        <v>12.5</v>
+        <v>6.858</v>
       </c>
       <c r="D16" t="n">
-        <v>0.3944</v>
+        <v>0.7477</v>
       </c>
     </row>
     <row r="17">
@@ -967,13 +987,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-10.5861</v>
+        <v>2.392</v>
       </c>
       <c r="C17" t="n">
-        <v>12.8267</v>
+        <v>6.8839</v>
       </c>
       <c r="D17" t="n">
-        <v>0.4092</v>
+        <v>0.7282</v>
       </c>
     </row>
     <row r="18">
@@ -981,13 +1001,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-9.9481</v>
+        <v>2.7592</v>
       </c>
       <c r="C18" t="n">
-        <v>12.7392</v>
+        <v>6.9302</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4349</v>
+        <v>0.6905</v>
       </c>
     </row>
     <row r="19">
@@ -995,13 +1015,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-9.8913</v>
+        <v>2.1065</v>
       </c>
       <c r="C19" t="n">
-        <v>12.7469</v>
+        <v>6.9411</v>
       </c>
       <c r="D19" t="n">
-        <v>0.4378</v>
+        <v>0.7615</v>
       </c>
     </row>
     <row r="20">
@@ -1009,13 +1029,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-9.545</v>
+        <v>0.9034</v>
       </c>
       <c r="C20" t="n">
-        <v>12.755</v>
+        <v>7.1055</v>
       </c>
       <c r="D20" t="n">
-        <v>0.4543</v>
+        <v>0.8988</v>
       </c>
     </row>
     <row r="21">
@@ -1023,13 +1043,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-9.8953</v>
+        <v>-0.3053</v>
       </c>
       <c r="C21" t="n">
-        <v>12.8016</v>
+        <v>7.79</v>
       </c>
       <c r="D21" t="n">
-        <v>0.4395</v>
+        <v>0.9687</v>
       </c>
     </row>
     <row r="22">
@@ -1037,13 +1057,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-10.2585</v>
+        <v>-1.5141</v>
       </c>
       <c r="C22" t="n">
-        <v>13.2301</v>
+        <v>9.2468</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4381</v>
+        <v>0.8699</v>
       </c>
     </row>
     <row r="23">
@@ -1051,13 +1071,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.6258</v>
+        <v>-0.6111</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1822</v>
+        <v>0.1794</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0006</v>
+        <v>0.0007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>